<commit_message>
locker and seatNumber bug fixed e.g in one locker only one student will be...
</commit_message>
<xml_diff>
--- a/backEnd/exportsStudentData/students_data.xlsx
+++ b/backEnd/exportsStudentData/students_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Registration Number</t>
   </si>
@@ -55,22 +55,22 @@
     <t>1</t>
   </si>
   <si>
-    <t>2025-03-03</t>
-  </si>
-  <si>
-    <t>testedit</t>
-  </si>
-  <si>
-    <t>testfathertest</t>
-  </si>
-  <si>
-    <t>testaddresstest</t>
-  </si>
-  <si>
-    <t>7250585055</t>
-  </si>
-  <si>
-    <t>22:00-06:00</t>
+    <t>2025-03-07</t>
+  </si>
+  <si>
+    <t>nikhil</t>
+  </si>
+  <si>
+    <t>kjkhuhuj</t>
+  </si>
+  <si>
+    <t>nghkk</t>
+  </si>
+  <si>
+    <t>8651993323</t>
+  </si>
+  <si>
+    <t>06:00-10:00, 22:00-06:00</t>
   </si>
   <si>
     <t>2</t>
@@ -79,37 +79,34 @@
     <t>350.00</t>
   </si>
   <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2025-03-02</t>
+    <t>50.00</t>
   </si>
   <si>
     <t>2025-03-08</t>
   </si>
   <si>
-    <t>testforfeesdues</t>
-  </si>
-  <si>
-    <t>testfather</t>
-  </si>
-  <si>
-    <t>testaddress</t>
-  </si>
-  <si>
-    <t>7250585051</t>
-  </si>
-  <si>
-    <t>06:00-10:00</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>2025-03-06</t>
+    <t>2025-02-05</t>
+  </si>
+  <si>
+    <t>satyam</t>
+  </si>
+  <si>
+    <t>ramkrishnanagar</t>
+  </si>
+  <si>
+    <t>7250585057</t>
+  </si>
+  <si>
+    <t>10:00-14:00, 14:00-18:00</t>
+  </si>
+  <si>
+    <t>400.00</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>2025-03-12</t>
   </si>
 </sst>
 </file>
@@ -567,7 +564,7 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
         <v>21</v>
@@ -576,10 +573,10 @@
         <v>22</v>
       </c>
       <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
         <v>23</v>
-      </c>
-      <c r="M2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -587,40 +584,40 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Home Page ui made look great
</commit_message>
<xml_diff>
--- a/backEnd/exportsStudentData/students_data.xlsx
+++ b/backEnd/exportsStudentData/students_data.xlsx
@@ -55,58 +55,58 @@
     <t>1</t>
   </si>
   <si>
-    <t>2025-03-07</t>
-  </si>
-  <si>
-    <t>nikhil</t>
-  </si>
-  <si>
-    <t>kjkhuhuj</t>
-  </si>
-  <si>
-    <t>nghkk</t>
-  </si>
-  <si>
-    <t>8651993323</t>
+    <t>2025-03-12</t>
+  </si>
+  <si>
+    <t>satyam</t>
+  </si>
+  <si>
+    <t>babu ji</t>
+  </si>
+  <si>
+    <t>ramkrishnanagar</t>
+  </si>
+  <si>
+    <t>7250585057</t>
   </si>
   <si>
     <t>06:00-10:00, 22:00-06:00</t>
   </si>
   <si>
+    <t>350.00</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>2025-04-12</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>350.00</t>
-  </si>
-  <si>
-    <t>50.00</t>
-  </si>
-  <si>
-    <t>2025-03-08</t>
-  </si>
-  <si>
-    <t>2025-02-05</t>
-  </si>
-  <si>
-    <t>satyam</t>
-  </si>
-  <si>
-    <t>ramkrishnanagar</t>
-  </si>
-  <si>
-    <t>7250585057</t>
-  </si>
-  <si>
-    <t>10:00-14:00, 14:00-18:00</t>
-  </si>
-  <si>
-    <t>400.00</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
-    <t>2025-03-12</t>
+    <t>2025-02-11</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testfather</t>
+  </si>
+  <si>
+    <t>7250585058</t>
+  </si>
+  <si>
+    <t>10:00-14:00</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2025-03-06</t>
   </si>
 </sst>
 </file>
@@ -561,27 +561,27 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
       </c>
       <c r="L2" t="s">
         <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -590,10 +590,10 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
@@ -602,19 +602,19 @@
         <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
       </c>
       <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
       </c>
       <c r="M3" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
everytheing is done only Testing is left
</commit_message>
<xml_diff>
--- a/backEnd/exportsStudentData/students_data.xlsx
+++ b/backEnd/exportsStudentData/students_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Registration Number</t>
   </si>
@@ -79,13 +79,13 @@
     <t>10.00</t>
   </si>
   <si>
-    <t>2025-04-12</t>
+    <t>2025-03-03</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>2025-02-11</t>
+    <t>2025-02-03</t>
   </si>
   <si>
     <t>test</t>
@@ -94,6 +94,9 @@
     <t>testfather</t>
   </si>
   <si>
+    <t>testaddress</t>
+  </si>
+  <si>
     <t>7250585058</t>
   </si>
   <si>
@@ -103,10 +106,37 @@
     <t>11.00</t>
   </si>
   <si>
+    <t>2025-03-13</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
-    <t>2025-03-06</t>
+    <t>2025-01-01</t>
+  </si>
+  <si>
+    <t>ashish</t>
+  </si>
+  <si>
+    <t>ashish ke babuji</t>
+  </si>
+  <si>
+    <t>7250585059</t>
+  </si>
+  <si>
+    <t>06:00-10:00</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>150.00</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2025-02-14</t>
   </si>
 </sst>
 </file>
@@ -483,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -593,13 +623,13 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -611,13 +641,54 @@
         <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="M3" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added forgot password functionality to send otp on given email and on that email only password reset happen
</commit_message>
<xml_diff>
--- a/backEnd/exportsStudentData/students_data.xlsx
+++ b/backEnd/exportsStudentData/students_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Registration Number</t>
   </si>
@@ -55,88 +55,34 @@
     <t>1</t>
   </si>
   <si>
-    <t>2025-03-12</t>
+    <t>2025-01-01</t>
   </si>
   <si>
     <t>satyam</t>
   </si>
   <si>
-    <t>babu ji</t>
+    <t>testfather</t>
   </si>
   <si>
     <t>ramkrishnanagar</t>
   </si>
   <si>
-    <t>7250585057</t>
+    <t>7250585058</t>
   </si>
   <si>
     <t>06:00-10:00, 22:00-06:00</t>
   </si>
   <si>
+    <t>1,2</t>
+  </si>
+  <si>
     <t>350.00</t>
   </si>
   <si>
-    <t>10.00</t>
-  </si>
-  <si>
-    <t>2025-03-03</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>2025-02-03</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>testfather</t>
-  </si>
-  <si>
-    <t>testaddress</t>
-  </si>
-  <si>
-    <t>7250585058</t>
-  </si>
-  <si>
-    <t>10:00-14:00</t>
-  </si>
-  <si>
-    <t>11.00</t>
-  </si>
-  <si>
-    <t>2025-03-13</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2025-01-01</t>
-  </si>
-  <si>
-    <t>ashish</t>
-  </si>
-  <si>
-    <t>ashish ke babuji</t>
-  </si>
-  <si>
-    <t>7250585059</t>
-  </si>
-  <si>
-    <t>06:00-10:00</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>150.00</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>2025-02-14</t>
+    <t>2025-03-05</t>
   </si>
 </sst>
 </file>
@@ -513,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -591,104 +537,22 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
         <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
everyfeature is working now only need to do regres tesing once
</commit_message>
<xml_diff>
--- a/backEnd/exportsStudentData/students_data.xlsx
+++ b/backEnd/exportsStudentData/students_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Registration Number</t>
   </si>
@@ -52,37 +52,100 @@
     <t>Fees Paid Till Date</t>
   </si>
   <si>
+    <t>Payment Mode</t>
+  </si>
+  <si>
+    <t>Admission Amount</t>
+  </si>
+  <si>
+    <t>Payment Expected Date</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2025-01-01</t>
+  </si>
+  <si>
+    <t>satyam</t>
+  </si>
+  <si>
+    <t>satyam ke papa</t>
+  </si>
+  <si>
+    <t>ramkrishnanagar</t>
+  </si>
+  <si>
+    <t>7250585057</t>
+  </si>
+  <si>
+    <t>22:00-06:00</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>350.00</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>2025-02-02</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>2025-03-23</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>2025-01-01</t>
-  </si>
-  <si>
-    <t>satyam</t>
+    <t>2025-01-02</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
   <si>
     <t>testfather</t>
   </si>
   <si>
-    <t>ramkrishnanagar</t>
-  </si>
-  <si>
     <t>7250585058</t>
   </si>
   <si>
-    <t>06:00-10:00, 22:00-06:00</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>350.00</t>
+    <t>06:00-10:00</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>2025-03-22</t>
+  </si>
+  <si>
+    <t>2025-03-01</t>
+  </si>
+  <si>
+    <t>testAgain</t>
+  </si>
+  <si>
+    <t>7250585051</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>150.00</t>
   </si>
   <si>
-    <t>2025-03-05</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2025-03-27</t>
   </si>
 </sst>
 </file>
@@ -459,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:P4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -471,9 +534,11 @@
     <col min="8" max="9" width="10" customWidth="1"/>
     <col min="10" max="12" width="15" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="15" width="15" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -513,46 +578,161 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>